<commit_message>
Correcciones menores a la escaleta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion02/Escaleta_CN_08_02_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion02/Escaleta_CN_08_02_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Edición\Amanda Varela\CN_08_02_CO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
@@ -11,14 +16,14 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$25</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="237">
   <si>
     <t>Asignatura</t>
   </si>
@@ -405,9 +410,6 @@
     <t>Interactivo que aborda los aspectos básicos del sistema endocrino</t>
   </si>
   <si>
-    <t>Actividad para reforzar la comprensión de los aspectos fundamentales del sistema endocrino</t>
-  </si>
-  <si>
     <t>Preguntas sobre la funcion del sistema endocrino.</t>
   </si>
   <si>
@@ -423,18 +425,9 @@
     <t>Los tipos de hormonas y su funcionamiento</t>
   </si>
   <si>
-    <t>Interactivo que explica diferentes aspectos sobre las hormonas</t>
-  </si>
-  <si>
-    <t>Animación que muestra algunas hormonas humanas importantes y explica su función en el cuerpo</t>
-  </si>
-  <si>
     <t>Cambiar el acento del audio</t>
   </si>
   <si>
-    <t>Primer menú explica la función de s. endocrino. La segunda explica en términos muy generales que son las hormonas. Usar ejemplo de adrenalina. La tercera explica muy por encima qué son glándulas Ejemplificar con las suprarrenales. Como hormonas y glándulas se explican más adelante, este es un recurso sencillo.</t>
-  </si>
-  <si>
     <t>Generalidades del sistema endocrino</t>
   </si>
   <si>
@@ -447,9 +440,6 @@
     <t>Refuerza tu aprendizaje: La función del sistema endocrino</t>
   </si>
   <si>
-    <t>Actividad acerca de las hormonas, sus funciones y sus mecanismos asociados</t>
-  </si>
-  <si>
     <t>Hacer preguntas o frases a completar con palabras como inhibición, retroalimentación, etc.</t>
   </si>
   <si>
@@ -459,24 +449,12 @@
     <t>Refuerza tu aprendizaje: Las hormonas y sus efectos</t>
   </si>
   <si>
-    <t>Actividad para reforzar la comprensión de las hormonas y su accionar</t>
-  </si>
-  <si>
     <t>La actividad de las hormonas</t>
   </si>
   <si>
     <t>Las glándulas</t>
   </si>
   <si>
-    <t>Interactivo que explica qué son las glándulas y muestra algunas de las más importantes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un primer menú explica qué son las glándulas endocrinas (y menciona brevemente las exocrinas). Los siguientes menús tratan sobre glándla simportantes, explicando su ubicación, las hormonas más importantes que producen, y la acción de dichas hormonas. </t>
-  </si>
-  <si>
-    <t>Interactivo con animación acerca de las glándulas del cuerpo humano</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -486,18 +464,9 @@
     <t>Las glándulas exocrinas y endocrinas</t>
   </si>
   <si>
-    <t>Actividad que relaciona algunas glándulas endocrinas importantes y las hormonas que producen</t>
-  </si>
-  <si>
-    <t>Actividad que trata sobre algunas glándulas endocrinas humanas importantes</t>
-  </si>
-  <si>
     <t>Relacionar glándulas con hormonas, con base en los ejemplos usados en los recursos expositivos de este guion</t>
   </si>
   <si>
-    <t>Los glándulas del sistema endocrino</t>
-  </si>
-  <si>
     <t>Preguntas variadas sobre las glándulas humanas expuestas en el recurso "Las glándulas del sistema endocrino". No preguntar detalles demasiado específicos.</t>
   </si>
   <si>
@@ -525,9 +494,6 @@
     <t>Las glándulas endocrinas humanas</t>
   </si>
   <si>
-    <t>Actividad para reforzar la comprensión de las glándulas endocrinas</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las glándulas productoras de hormonas</t>
   </si>
   <si>
@@ -540,33 +506,21 @@
     <t>Refuerza tu aprendizaje: Las enfermedades del sistema endocrino</t>
   </si>
   <si>
-    <t>Actividad para reforzar la comprensión de las alteraciones del sistema endocrino</t>
-  </si>
-  <si>
     <t>Sustancias que alteran el sistema endocrino</t>
   </si>
   <si>
-    <t>Actividad que trata sobre los alteradores endocrinos</t>
-  </si>
-  <si>
     <t>Se hace un texto sobre alteradores endocrinos, mencionando las formas en las que pueden alterar el sistema y algunos ejemplos</t>
   </si>
   <si>
     <t>Enfermedades derivadas de cambios en la actividad de las glándulas</t>
   </si>
   <si>
-    <t>Actividad para reconocer alteraciones del sistema endocrino debidas a cambios en el tamaño de las glándulas</t>
-  </si>
-  <si>
     <t>Enfermedades derivadas de cambios en el tamaño de las glándulas</t>
   </si>
   <si>
     <t>Las enfermedades del sistema endocrino</t>
   </si>
   <si>
-    <t>Interactivo que trata sobre alteraciones en las glándulas endocrinas</t>
-  </si>
-  <si>
     <t>Describir efectos de diferentes enfermedades, para llevar al contenedor correspondiente. Hiperplasia benigna de próstata, Bocio, Bartolinitis.</t>
   </si>
   <si>
@@ -594,18 +548,6 @@
     <t>Evaluación</t>
   </si>
   <si>
-    <t>Banco de actividades: La ciencia detrás de las comunicaciones</t>
-  </si>
-  <si>
-    <t>Mapa conceptual del tema La ciencia detrás de las comunicaciones</t>
-  </si>
-  <si>
-    <t>Evalúa tus conocimientos acerca del tema La ciencia detrás de las comunicaciones </t>
-  </si>
-  <si>
-    <t>Motor que incluye preguntas de respuesta abierta del tema La ciencia detrás de las comunicaciones</t>
-  </si>
-  <si>
     <t>RM</t>
   </si>
   <si>
@@ -727,6 +669,72 @@
   </si>
   <si>
     <t>Recurso M101A-04</t>
+  </si>
+  <si>
+    <t>Banco de actividades: El sistema endocrino</t>
+  </si>
+  <si>
+    <t>Motor que incluye preguntas de respuesta abierta del tema El sistema endocrino</t>
+  </si>
+  <si>
+    <t>Evalúa tus conocimientos acerca del tema El sistema endocrino</t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema El sistema endocrino</t>
+  </si>
+  <si>
+    <t>Las glándulas del sistema endocrino</t>
+  </si>
+  <si>
+    <t>Un primer menú explica qué son las glándulas endocrinas (y menciona brevemente las exocrinas). Los siguientes menús tratan sobre glándulas importantes, explicando su ubicación, las hormonas más importantes que producen, y la acción de dichas hormonas.</t>
+  </si>
+  <si>
+    <t>Actividad para identificar algunas glándulas endocrinas humanas importantes y reconocer su función</t>
+  </si>
+  <si>
+    <t>Actividad para analizar las funciones de las glándulas endocrinas</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer alteraciones del sistema endocrino debidas a cambios en la actividad de las glándulas</t>
+  </si>
+  <si>
+    <t>Actividad para analizar diversos aspectos sobre las alteraciones del sistema endocrino</t>
+  </si>
+  <si>
+    <t>Actividad para analizar aspectos fundamentales del sistema endocrino</t>
+  </si>
+  <si>
+    <t>Interactivo para diferenciar los tipos de hormonas que existen, y comprender como se da su liberación captación y regulación, así como sus efectos en el organismo</t>
+  </si>
+  <si>
+    <t>Animación para conocer algunas hormonas humanas importantes y entender su función en el organismo</t>
+  </si>
+  <si>
+    <t>Actividad para recordar diversos aspectos relativos a las hormonas</t>
+  </si>
+  <si>
+    <t>Actividad para analizar la función y regulación hormonal</t>
+  </si>
+  <si>
+    <t>Interactivo para comprender qué son las glándulas y reconocer algunas de las más importantes</t>
+  </si>
+  <si>
+    <t>Interactivo con animación para reconocer algunas de las principales glándulas del cuerpo humano</t>
+  </si>
+  <si>
+    <t>Actividad para relacionar algunas glándulas endocrinas importantes con las hormonas que producen</t>
+  </si>
+  <si>
+    <t>Interactivo para comprender y diferenciar las posibles alteraciones en las glándulas endocrinas</t>
+  </si>
+  <si>
+    <t>Actividad para relacionar enfermedades con alteraciones del sistema endocrino debidas a cambios en el tamaño de las glándulas</t>
+  </si>
+  <si>
+    <t>Actividad para repasar lo aprendido sobre alteradores endocrinos</t>
+  </si>
+  <si>
+    <t>Primer menú explica la función del s. endocrino. La segunda explica en términos muy generales que son las hormonas. Usar ejemplo de adrenalina. La tercera explica muy por encima qué son glándulas Ejemplificar con las suprarrenales. Como hormonas y glándulas se explican más adelante, este es un recurso sencillo.</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1075,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1102,7 +1110,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1313,9 +1321,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T20" sqref="T20"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1478,7 @@
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="9" t="s">
-        <v>137</v>
+        <v>236</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>19</v>
@@ -1479,16 +1487,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="T3" s="21" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1507,7 +1515,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="9"/>
       <c r="G4" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1516,7 +1524,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>19</v>
@@ -1527,25 +1535,25 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="U4" s="19" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1566,7 +1574,7 @@
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H5" s="9">
         <v>3</v>
@@ -1575,7 +1583,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>20</v>
@@ -1588,7 +1596,7 @@
         <v>52</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P5" s="9" t="s">
         <v>19</v>
@@ -1597,16 +1605,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1620,12 +1628,12 @@
         <v>123</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="9"/>
       <c r="G6" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H6" s="9">
         <v>4</v>
@@ -1634,7 +1642,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>134</v>
+        <v>226</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1647,7 +1655,7 @@
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P6" s="9" t="s">
         <v>19</v>
@@ -1656,16 +1664,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1679,14 +1687,14 @@
         <v>123</v>
       </c>
       <c r="D7" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>131</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>132</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="16" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -1695,7 +1703,7 @@
         <v>19</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>135</v>
+        <v>227</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -1706,25 +1714,25 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
       <c r="O7" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1738,14 +1746,14 @@
         <v>123</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="16" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H8" s="9">
         <v>6</v>
@@ -1754,7 +1762,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>142</v>
+        <v>228</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>20</v>
@@ -1767,7 +1775,7 @@
         <v>120</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="P8" s="9" t="s">
         <v>19</v>
@@ -1776,16 +1784,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1799,14 +1807,14 @@
         <v>123</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="16" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="H9" s="9">
         <v>7</v>
@@ -1815,7 +1823,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>20</v>
@@ -1828,25 +1836,25 @@
         <v>32</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="Q9" s="10">
         <v>6</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1860,14 +1868,14 @@
         <v>123</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>125</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -1876,7 +1884,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>146</v>
+        <v>229</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>20</v>
@@ -1889,7 +1897,7 @@
         <v>52</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -1898,16 +1906,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1921,12 +1929,12 @@
         <v>123</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="9"/>
       <c r="G11" s="16" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="H11" s="9">
         <v>9</v>
@@ -1935,7 +1943,7 @@
         <v>19</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>20</v>
@@ -1948,7 +1956,7 @@
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="9" t="s">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="P11" s="9" t="s">
         <v>19</v>
@@ -1957,16 +1965,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="T11" s="12" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1980,12 +1988,12 @@
         <v>123</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="9"/>
       <c r="G12" s="16" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H12" s="9">
         <v>10</v>
@@ -1994,7 +2002,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>151</v>
+        <v>231</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>19</v>
@@ -2005,25 +2013,25 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q12" s="10" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2037,14 +2045,14 @@
         <v>123</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="16" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2053,7 +2061,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>155</v>
+        <v>232</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2066,7 +2074,7 @@
         <v>23</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>19</v>
@@ -2075,16 +2083,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2098,14 +2106,14 @@
         <v>123</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="16" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="H14" s="9">
         <v>12</v>
@@ -2114,7 +2122,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>156</v>
+        <v>221</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2127,25 +2135,25 @@
         <v>32</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="Q14" s="10">
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2159,14 +2167,14 @@
         <v>123</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>125</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="H15" s="9">
         <v>13</v>
@@ -2175,7 +2183,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2189,22 +2197,22 @@
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="Q15" s="10">
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2218,12 +2226,12 @@
         <v>123</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="9"/>
       <c r="G16" s="16" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2232,7 +2240,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2245,7 +2253,7 @@
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="9" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2254,16 +2262,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2277,14 +2285,14 @@
         <v>123</v>
       </c>
       <c r="D17" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>171</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>188</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="16" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="H17" s="9">
         <v>15</v>
@@ -2293,7 +2301,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>178</v>
+        <v>234</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2306,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2315,16 +2323,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2338,14 +2346,14 @@
         <v>123</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="16" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="H18" s="9">
         <v>16</v>
@@ -2354,7 +2362,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="17" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>19</v>
@@ -2369,19 +2377,19 @@
         <v>19</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2395,14 +2403,14 @@
         <v>123</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="16" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2411,7 +2419,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>175</v>
+        <v>235</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2424,7 +2432,7 @@
         <v>28</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
@@ -2433,16 +2441,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2456,14 +2464,14 @@
         <v>123</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="16" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="H20" s="9">
         <v>18</v>
@@ -2472,7 +2480,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>173</v>
+        <v>224</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2492,16 +2500,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2515,12 +2523,12 @@
         <v>123</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
@@ -2529,7 +2537,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2542,7 +2550,7 @@
         <v>121</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>19</v>
@@ -2551,16 +2559,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2574,12 +2582,12 @@
         <v>123</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="H22" s="9">
         <v>20</v>
@@ -2588,7 +2596,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2601,7 +2609,7 @@
         <v>121</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>19</v>
@@ -2610,16 +2618,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2633,7 +2641,7 @@
         <v>123</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="9"/>
@@ -2647,7 +2655,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2678,12 +2686,12 @@
         <v>123</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="H24" s="9">
         <v>22</v>
@@ -2692,7 +2700,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2712,16 +2720,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2735,12 +2743,12 @@
         <v>123</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="H25" s="9">
         <v>23</v>
@@ -2749,7 +2757,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2769,16 +2777,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4316,7 +4324,7 @@
     <row r="289" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
     <row r="290" ht="14.45" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <autoFilter ref="A1:U2">
+  <autoFilter ref="A1:U25">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">

</xml_diff>